<commit_message>
Make servo pull faster
</commit_message>
<xml_diff>
--- a/Doc/JedEye PuppetMaster plan.xlsx
+++ b/Doc/JedEye PuppetMaster plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>done</t>
   </si>
@@ -94,18 +94,6 @@
     <t>create movement segments</t>
   </si>
   <si>
-    <t>dance around with the puppet to make it more appealing to viewers</t>
-  </si>
-  <si>
-    <t>find proper music for the puppet's performance</t>
-  </si>
-  <si>
-    <t>sing along with the music to attract female conference attendants</t>
-  </si>
-  <si>
-    <t>dress up as puppets for a more immersing viewing experience</t>
-  </si>
-  <si>
     <t>make basic reading of pressure values into data structure</t>
   </si>
   <si>
@@ -113,6 +101,9 @@
   </si>
   <si>
     <t>prepare and test plan for disassembly and reassembly of hardware</t>
+  </si>
+  <si>
+    <t>make the servo pull string faster</t>
   </si>
 </sst>
 </file>
@@ -514,7 +505,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +540,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -563,7 +554,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -597,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -609,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -619,7 +610,7 @@
       </c>
       <c r="B9" s="1"/>
       <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -629,7 +620,7 @@
       </c>
       <c r="B10" s="1"/>
       <c r="G10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -639,7 +630,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="G11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -649,7 +640,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -659,7 +650,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="G13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -669,7 +660,7 @@
       </c>
       <c r="B14" s="1"/>
       <c r="G14" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -678,9 +669,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="G15" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -688,9 +677,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="G16" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -698,9 +685,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="G17" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>